<commit_message>
added batch FSH investigation
</commit_message>
<xml_diff>
--- a/hw_global/Data/hourlyDataSchema.xlsx
+++ b/hw_global/Data/hourlyDataSchema.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="146">
   <si>
     <t xml:space="preserve">Variable</t>
   </si>
@@ -392,6 +392,9 @@
   </si>
   <si>
     <t xml:space="preserve">urban heating flux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zero importance</t>
   </si>
   <si>
     <t xml:space="preserve">VAPOR_PRES</t>
@@ -464,7 +467,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -493,6 +496,12 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="3">
@@ -543,7 +552,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -557,6 +566,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -639,15 +652,15 @@
   </sheetPr>
   <dimension ref="A1:L59"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K52" activeCellId="0" sqref="K52"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I47" activeCellId="0" sqref="I47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="66.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="61.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="78.08"/>
   </cols>
@@ -1221,7 +1234,9 @@
       <c r="G23" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H23" s="2"/>
+      <c r="H23" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="I23" s="3" t="s">
         <v>34</v>
       </c>
@@ -1923,18 +1938,21 @@
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="0" t="s">
-        <v>34</v>
+        <v>61</v>
+      </c>
+      <c r="K50" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>88</v>
@@ -1955,18 +1973,18 @@
         <v>61</v>
       </c>
       <c r="K51" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>88</v>
@@ -1984,13 +2002,13 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>88</v>
@@ -2008,13 +2026,13 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>33</v>
@@ -2032,13 +2050,13 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>25</v>
@@ -2055,13 +2073,13 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>25</v>
@@ -2076,18 +2094,18 @@
         <v>14</v>
       </c>
       <c r="I56" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>25</v>
@@ -2102,18 +2120,18 @@
         <v>14</v>
       </c>
       <c r="I57" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>121</v>
@@ -2131,16 +2149,16 @@
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="I59" s="0" t="s">
         <v>34</v>
       </c>
       <c r="K59" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>